<commit_message>
trying to ignore file
</commit_message>
<xml_diff>
--- a/excel1.xlsx
+++ b/excel1.xlsx
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>vsd;oa;</t>
+  </si>
+  <si>
+    <t>fkeop34opf4f</t>
   </si>
 </sst>
 </file>
@@ -350,15 +353,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="C5" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>